<commit_message>
bottom nav bar with selection
</commit_message>
<xml_diff>
--- a/Documentation/Reports/TimeReport_SabrinaLuu.xlsx
+++ b/Documentation/Reports/TimeReport_SabrinaLuu.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sabrina\Documents\cped1\plant_partner\plant-partner\Documentation\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27B74637-DBDF-4449-96A7-26D6050AC5FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79042879-D542-4EB7-8DBF-367DA3C271AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{605B5A91-C2DF-4ED5-9E2C-366EB894E8F1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
     <t>Name:</t>
   </si>
@@ -90,6 +90,21 @@
   </si>
   <si>
     <t>Addressed comments and critiques on design draft, revised interfaces with labels, more descriptions for storyboarding.</t>
+  </si>
+  <si>
+    <t>Research</t>
+  </si>
+  <si>
+    <t>Check-in: Group meetign with Tyler, discussed what was needed for the pre-alpha build, planning more research for app development</t>
+  </si>
+  <si>
+    <t>Researching how to implement and use Flutter in conjunction with MongoDB, watching tutorials on how to use Dart</t>
+  </si>
+  <si>
+    <t>Group Work</t>
+  </si>
+  <si>
+    <t>Starting to add backend/frontend modules</t>
   </si>
 </sst>
 </file>
@@ -657,8 +672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25321167-01B1-413D-AB29-4165F3CF20BA}">
   <dimension ref="A1:F199"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -683,7 +698,7 @@
       </c>
       <c r="E1" s="6">
         <f>SUM(E4:E199)</f>
-        <v>0.47500000000000014</v>
+        <v>-9.097222222222201E-2</v>
       </c>
       <c r="F1" s="17"/>
     </row>
@@ -764,7 +779,7 @@
         <v>0.64722222222222225</v>
       </c>
       <c r="E6" s="10">
-        <f t="shared" ref="E5:E68" si="0">D6-C6</f>
+        <f t="shared" ref="E6:E68" si="0">D6-C6</f>
         <v>2.2222222222222254E-2</v>
       </c>
       <c r="F6" s="15" t="s">
@@ -813,37 +828,65 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="7"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
+      <c r="A9" s="7">
+        <v>45950</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="9">
+        <v>0.625</v>
+      </c>
+      <c r="D9" s="9">
+        <v>0.64722222222222225</v>
+      </c>
       <c r="E9" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F9" s="15"/>
+        <v>2.2222222222222254E-2</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="7"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
+      <c r="A10" s="7">
+        <v>45954</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="9">
+        <v>0.5229166666666667</v>
+      </c>
+      <c r="D10" s="9">
+        <v>0.55694444444444446</v>
+      </c>
       <c r="E10" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F10" s="15"/>
+        <v>3.4027777777777768E-2</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="11"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
+      <c r="A11" s="7">
+        <v>45954</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="9">
+        <v>0.62222222222222223</v>
+      </c>
       <c r="D11" s="8"/>
       <c r="E11" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F11" s="15"/>
+        <v>-0.62222222222222223</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="11"/>

</xml_diff>

<commit_message>
main bottom nav pages done, tasks, home, settings
</commit_message>
<xml_diff>
--- a/Documentation/Reports/TimeReport_SabrinaLuu.xlsx
+++ b/Documentation/Reports/TimeReport_SabrinaLuu.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sabrina\Documents\cped1\plant_partner\plant-partner\Documentation\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79042879-D542-4EB7-8DBF-367DA3C271AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9598DC82-E4B1-4A09-A8FC-78A8B9F00F40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{605B5A91-C2DF-4ED5-9E2C-366EB894E8F1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
   <si>
     <t>Name:</t>
   </si>
@@ -104,7 +104,10 @@
     <t>Group Work</t>
   </si>
   <si>
-    <t>Starting to add backend/frontend modules</t>
+    <t>,</t>
+  </si>
+  <si>
+    <t>Fully set up Flutter and Dart, using the Android Emulator to simulate front end changes, implemented custom bottom navigation bar</t>
   </si>
 </sst>
 </file>
@@ -670,7 +673,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25321167-01B1-413D-AB29-4165F3CF20BA}">
-  <dimension ref="A1:F199"/>
+  <dimension ref="A1:G199"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
@@ -686,7 +689,7 @@
     <col min="6" max="6" width="163" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -702,8 +705,8 @@
       </c>
       <c r="F1" s="17"/>
     </row>
-    <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -723,7 +726,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>45933</v>
       </c>
@@ -744,7 +747,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>11</v>
       </c>
@@ -765,7 +768,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>45936</v>
       </c>
@@ -786,7 +789,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>45944</v>
       </c>
@@ -807,7 +810,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>45949</v>
       </c>
@@ -827,7 +830,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>45950</v>
       </c>
@@ -848,7 +851,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>45954</v>
       </c>
@@ -869,7 +872,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="7">
         <v>45954</v>
       </c>
@@ -885,10 +888,13 @@
         <v>-0.62222222222222223</v>
       </c>
       <c r="F11" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="11"/>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
@@ -899,7 +905,7 @@
       </c>
       <c r="F12" s="15"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="11"/>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
@@ -910,7 +916,7 @@
       </c>
       <c r="F13" s="15"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="11"/>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
@@ -921,7 +927,7 @@
       </c>
       <c r="F14" s="15"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="11"/>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
@@ -932,7 +938,7 @@
       </c>
       <c r="F15" s="15"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="11"/>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>

</xml_diff>

<commit_message>
update sab time, deleted my garbage in backend
</commit_message>
<xml_diff>
--- a/Documentation/Reports/TimeReport_SabrinaLuu.xlsx
+++ b/Documentation/Reports/TimeReport_SabrinaLuu.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sabrina\Documents\cped1\plant_partner\plant-partner\Documentation\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9598DC82-E4B1-4A09-A8FC-78A8B9F00F40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{254C9437-37BE-4277-BB6D-9DD47A5457B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{605B5A91-C2DF-4ED5-9E2C-366EB894E8F1}"/>
   </bookViews>
@@ -107,7 +107,7 @@
     <t>,</t>
   </si>
   <si>
-    <t>Fully set up Flutter and Dart, using the Android Emulator to simulate front end changes, implemented custom bottom navigation bar</t>
+    <t>Fully set up Flutter and Dart, using the Android Emulator to simulate front end changes, implemented custom bottom navigation bar, creates basis 3 pages from the bottom nav bar</t>
   </si>
 </sst>
 </file>
@@ -675,8 +675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25321167-01B1-413D-AB29-4165F3CF20BA}">
   <dimension ref="A1:G199"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -701,7 +701,7 @@
       </c>
       <c r="E1" s="6">
         <f>SUM(E4:E199)</f>
-        <v>-9.097222222222201E-2</v>
+        <v>0.79097222222222241</v>
       </c>
       <c r="F1" s="17"/>
     </row>
@@ -882,10 +882,12 @@
       <c r="C11" s="9">
         <v>0.62222222222222223</v>
       </c>
-      <c r="D11" s="8"/>
+      <c r="D11" s="9">
+        <v>0.88194444444444442</v>
+      </c>
       <c r="E11" s="10">
         <f t="shared" si="0"/>
-        <v>-0.62222222222222223</v>
+        <v>0.25972222222222219</v>
       </c>
       <c r="F11" s="15" t="s">
         <v>23</v>

</xml_diff>